<commit_message>
Documentation: added README to Resources and cleaned up details in UniversalGazetteerModel.xlsx
</commit_message>
<xml_diff>
--- a/GazetteerETL/Resources/USGSCountryAdjusts.xlsx
+++ b/GazetteerETL/Resources/USGSCountryAdjusts.xlsx
@@ -8,11 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$1:$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$15</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -453,7 +451,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,33 +627,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XEX16"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <autoFilter ref="A1:C15"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>